<commit_message>
08.07.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/July/Others/Allocation Sheet.xlsx
+++ b/July/Others/Allocation Sheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="104">
   <si>
     <t>BL60</t>
   </si>
@@ -321,6 +321,12 @@
   </si>
   <si>
     <t>DSR NAME:   Md Shohel Rana</t>
+  </si>
+  <si>
+    <t>Robiul: 01751-312831</t>
+  </si>
+  <si>
+    <t>DSR NAME:   Md Robiul Islam</t>
   </si>
 </sst>
 </file>
@@ -330,7 +336,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,13 +370,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Bauhaus 93"/>
-      <family val="5"/>
     </font>
     <font>
       <b/>
@@ -435,7 +434,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -513,13 +512,75 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -534,50 +595,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -586,22 +623,10 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -617,16 +642,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -637,17 +653,74 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1019,6 +1092,94 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>29158</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>9719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38878</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>9720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Connector 7"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="29158" y="12287444"/>
+          <a:ext cx="2362395" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>194388</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9719</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>194390</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Connector 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7086601" y="12272088"/>
+          <a:ext cx="1524193" cy="2"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1310,7 +1471,7 @@
   <dimension ref="A1:O61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:O61"/>
+      <selection activeCell="O64" sqref="A1:O64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1332,73 +1493,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="43" t="s">
+      <c r="A1" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="44" t="s">
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-    </row>
-    <row r="3" spans="1:15" s="13" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="6" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+    </row>
+    <row r="3" spans="1:15" s="6" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A3" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1406,63 +1567,63 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
+      <c r="L4" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="H5" s="16"/>
-      <c r="I5" s="15" t="s">
+      <c r="H5" s="8"/>
+      <c r="I5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="L5" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="M5" s="16" t="s">
+      <c r="M5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="16" t="s">
+      <c r="N5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="16" t="s">
+      <c r="O5" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="11">
         <v>800</v>
       </c>
       <c r="C6" s="4">
@@ -1473,10 +1634,10 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="J6" s="21">
+      <c r="J6" s="13">
         <v>5750</v>
       </c>
       <c r="K6" s="4">
@@ -1488,10 +1649,10 @@
       <c r="O6" s="4"/>
     </row>
     <row r="7" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="11">
         <v>780</v>
       </c>
       <c r="C7" s="4">
@@ -1502,10 +1663,10 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="J7" s="23">
+      <c r="J7" s="15">
         <v>4640</v>
       </c>
       <c r="K7" s="4">
@@ -1517,10 +1678,10 @@
       <c r="O7" s="4"/>
     </row>
     <row r="8" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="11">
         <v>865</v>
       </c>
       <c r="C8" s="4">
@@ -1531,10 +1692,10 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="10">
         <v>5650</v>
       </c>
       <c r="K8" s="4">
@@ -1546,10 +1707,10 @@
       <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="11">
         <v>810</v>
       </c>
       <c r="C9" s="4">
@@ -1560,10 +1721,10 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="18" t="s">
+      <c r="I9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="13">
         <v>5020</v>
       </c>
       <c r="K9" s="4">
@@ -1575,10 +1736,10 @@
       <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="11">
         <v>800</v>
       </c>
       <c r="C10" s="4">
@@ -1589,10 +1750,10 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="13">
         <v>5280</v>
       </c>
       <c r="K10" s="4">
@@ -1604,10 +1765,10 @@
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="11">
         <v>795</v>
       </c>
       <c r="C11" s="4">
@@ -1618,10 +1779,10 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="13">
         <v>4820</v>
       </c>
       <c r="K11" s="4">
@@ -1633,10 +1794,10 @@
       <c r="O11" s="4"/>
     </row>
     <row r="12" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="11">
         <v>790</v>
       </c>
       <c r="C12" s="4">
@@ -1647,10 +1808,10 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="18" t="s">
+      <c r="I12" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="J12" s="21">
+      <c r="J12" s="13">
         <v>5100</v>
       </c>
       <c r="K12" s="4">
@@ -1662,10 +1823,10 @@
       <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="11">
         <v>800</v>
       </c>
       <c r="C13" s="4">
@@ -1676,10 +1837,10 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="20" t="s">
+      <c r="I13" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="21">
+      <c r="J13" s="13">
         <v>5560</v>
       </c>
       <c r="K13" s="4">
@@ -1691,10 +1852,10 @@
       <c r="O13" s="4"/>
     </row>
     <row r="14" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="11">
         <v>970</v>
       </c>
       <c r="C14" s="4">
@@ -1705,10 +1866,10 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="18" t="s">
+      <c r="I14" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="J14" s="21">
+      <c r="J14" s="13">
         <v>6090</v>
       </c>
       <c r="K14" s="4">
@@ -1720,10 +1881,10 @@
       <c r="O14" s="4"/>
     </row>
     <row r="15" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="11">
         <v>900</v>
       </c>
       <c r="C15" s="4">
@@ -1734,10 +1895,10 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="20" t="s">
+      <c r="I15" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="J15" s="21">
+      <c r="J15" s="13">
         <v>5390</v>
       </c>
       <c r="K15" s="4">
@@ -1749,10 +1910,10 @@
       <c r="O15" s="4"/>
     </row>
     <row r="16" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="11">
         <v>915</v>
       </c>
       <c r="C16" s="4">
@@ -1763,10 +1924,10 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="20" t="s">
+      <c r="I16" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="J16" s="21">
+      <c r="J16" s="13">
         <v>3630</v>
       </c>
       <c r="K16" s="4">
@@ -1778,10 +1939,10 @@
       <c r="O16" s="4"/>
     </row>
     <row r="17" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="11">
         <v>910</v>
       </c>
       <c r="C17" s="4">
@@ -1792,10 +1953,10 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="18" t="s">
+      <c r="I17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J17" s="21">
+      <c r="J17" s="13">
         <v>3560</v>
       </c>
       <c r="K17" s="4">
@@ -1807,10 +1968,10 @@
       <c r="O17" s="4"/>
     </row>
     <row r="18" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="19">
+      <c r="B18" s="11">
         <v>890</v>
       </c>
       <c r="C18" s="4">
@@ -1821,10 +1982,10 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="18" t="s">
+      <c r="I18" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="J18" s="21">
+      <c r="J18" s="13">
         <v>3340</v>
       </c>
       <c r="K18" s="4">
@@ -1836,10 +1997,10 @@
       <c r="O18" s="4"/>
     </row>
     <row r="19" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="19">
+      <c r="B19" s="11">
         <v>920</v>
       </c>
       <c r="C19" s="4">
@@ -1850,10 +2011,10 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="20" t="s">
+      <c r="I19" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="J19" s="21">
+      <c r="J19" s="13">
         <v>5390</v>
       </c>
       <c r="K19" s="4">
@@ -1865,10 +2026,10 @@
       <c r="O19" s="4"/>
     </row>
     <row r="20" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="19">
+      <c r="B20" s="11">
         <v>880</v>
       </c>
       <c r="C20" s="4">
@@ -1879,10 +2040,10 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="18" t="s">
+      <c r="I20" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="J20" s="21">
+      <c r="J20" s="13">
         <v>4500</v>
       </c>
       <c r="K20" s="4">
@@ -1894,10 +2055,10 @@
       <c r="O20" s="4"/>
     </row>
     <row r="21" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="19">
+      <c r="B21" s="11">
         <v>1000</v>
       </c>
       <c r="C21" s="4">
@@ -1908,10 +2069,10 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
-      <c r="I21" s="18" t="s">
+      <c r="I21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="J21" s="21">
+      <c r="J21" s="13">
         <v>4970</v>
       </c>
       <c r="K21" s="4">
@@ -1923,10 +2084,10 @@
       <c r="O21" s="4"/>
     </row>
     <row r="22" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="19">
+      <c r="B22" s="11">
         <v>995</v>
       </c>
       <c r="C22" s="4">
@@ -1937,10 +2098,10 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
-      <c r="I22" s="18" t="s">
+      <c r="I22" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="J22" s="21">
+      <c r="J22" s="13">
         <v>4015</v>
       </c>
       <c r="K22" s="4">
@@ -1952,10 +2113,10 @@
       <c r="O22" s="4"/>
     </row>
     <row r="23" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="19">
+      <c r="B23" s="11">
         <v>1000</v>
       </c>
       <c r="C23" s="4">
@@ -1966,10 +2127,10 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="18" t="s">
+      <c r="I23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="21">
+      <c r="J23" s="13">
         <v>3710</v>
       </c>
       <c r="K23" s="4">
@@ -1981,10 +2142,10 @@
       <c r="O23" s="4"/>
     </row>
     <row r="24" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B24" s="11">
         <v>960</v>
       </c>
       <c r="C24" s="4">
@@ -1995,10 +2156,10 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="18" t="s">
+      <c r="I24" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="J24" s="21">
+      <c r="J24" s="13">
         <v>3620</v>
       </c>
       <c r="K24" s="4">
@@ -2010,10 +2171,10 @@
       <c r="O24" s="4"/>
     </row>
     <row r="25" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="11">
         <v>1040</v>
       </c>
       <c r="C25" s="4">
@@ -2024,10 +2185,10 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
-      <c r="I25" s="18" t="s">
+      <c r="I25" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J25" s="21">
+      <c r="J25" s="13">
         <v>4620</v>
       </c>
       <c r="K25" s="4">
@@ -2039,10 +2200,10 @@
       <c r="O25" s="4"/>
     </row>
     <row r="26" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B26" s="19">
+      <c r="B26" s="11">
         <v>930</v>
       </c>
       <c r="C26" s="4">
@@ -2053,10 +2214,10 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-      <c r="I26" s="18" t="s">
+      <c r="I26" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="J26" s="21">
+      <c r="J26" s="13">
         <v>4520</v>
       </c>
       <c r="K26" s="4">
@@ -2068,10 +2229,10 @@
       <c r="O26" s="4"/>
     </row>
     <row r="27" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="11">
         <v>1290</v>
       </c>
       <c r="C27" s="4">
@@ -2082,10 +2243,10 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
-      <c r="I27" s="18" t="s">
+      <c r="I27" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="J27" s="21">
+      <c r="J27" s="13">
         <v>4080</v>
       </c>
       <c r="K27" s="4">
@@ -2097,10 +2258,10 @@
       <c r="O27" s="4"/>
     </row>
     <row r="28" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B28" s="19">
+      <c r="B28" s="11">
         <v>1190</v>
       </c>
       <c r="C28" s="4">
@@ -2111,10 +2272,10 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
-      <c r="I28" s="22" t="s">
+      <c r="I28" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="J28" s="21">
+      <c r="J28" s="13">
         <v>4220</v>
       </c>
       <c r="K28" s="4">
@@ -2126,10 +2287,10 @@
       <c r="O28" s="4"/>
     </row>
     <row r="29" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="19">
+      <c r="B29" s="11">
         <v>1270</v>
       </c>
       <c r="C29" s="4">
@@ -2140,10 +2301,10 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
-      <c r="I29" s="22" t="s">
+      <c r="I29" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="J29" s="21">
+      <c r="J29" s="13">
         <v>12240</v>
       </c>
       <c r="K29" s="4">
@@ -2155,10 +2316,10 @@
       <c r="O29" s="4"/>
     </row>
     <row r="30" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="19">
+      <c r="B30" s="11">
         <v>1170</v>
       </c>
       <c r="C30" s="4">
@@ -2169,10 +2330,10 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
-      <c r="I30" s="18" t="s">
+      <c r="I30" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="J30" s="23">
+      <c r="J30" s="15">
         <v>12090</v>
       </c>
       <c r="K30" s="4">
@@ -2184,10 +2345,10 @@
       <c r="O30" s="4"/>
     </row>
     <row r="31" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="19">
+      <c r="B31" s="11">
         <v>1190</v>
       </c>
       <c r="C31" s="4">
@@ -2198,10 +2359,10 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
-      <c r="I31" s="20" t="s">
+      <c r="I31" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="J31" s="23">
+      <c r="J31" s="15">
         <v>10840</v>
       </c>
       <c r="K31" s="4">
@@ -2213,10 +2374,10 @@
       <c r="O31" s="4"/>
     </row>
     <row r="32" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B32" s="19">
+      <c r="B32" s="11">
         <v>1225</v>
       </c>
       <c r="C32" s="4">
@@ -2227,10 +2388,10 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
-      <c r="I32" s="20" t="s">
+      <c r="I32" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="J32" s="23">
+      <c r="J32" s="15">
         <v>12490</v>
       </c>
       <c r="K32" s="4">
@@ -2242,10 +2403,10 @@
       <c r="O32" s="4"/>
     </row>
     <row r="33" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="19">
+      <c r="B33" s="11">
         <v>1220</v>
       </c>
       <c r="C33" s="4">
@@ -2256,10 +2417,10 @@
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
-      <c r="I33" s="20" t="s">
+      <c r="I33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="J33" s="21">
+      <c r="J33" s="13">
         <v>8820</v>
       </c>
       <c r="K33" s="4">
@@ -2271,10 +2432,10 @@
       <c r="O33" s="4"/>
     </row>
     <row r="34" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="19">
+      <c r="B34" s="11">
         <v>1080</v>
       </c>
       <c r="C34" s="4">
@@ -2285,8 +2446,8 @@
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="23"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="15"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
@@ -2294,10 +2455,10 @@
       <c r="O34" s="4"/>
     </row>
     <row r="35" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="19">
+      <c r="B35" s="11">
         <v>1100</v>
       </c>
       <c r="C35" s="4">
@@ -2308,8 +2469,8 @@
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="21"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="13"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
@@ -2317,10 +2478,10 @@
       <c r="O35" s="4"/>
     </row>
     <row r="36" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="24">
+      <c r="B36" s="16">
         <v>1200</v>
       </c>
       <c r="C36" s="4">
@@ -2331,8 +2492,8 @@
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="21"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="13"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
@@ -2340,10 +2501,10 @@
       <c r="O36" s="4"/>
     </row>
     <row r="37" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="19">
+      <c r="B37" s="11">
         <v>1120</v>
       </c>
       <c r="C37" s="4">
@@ -2354,8 +2515,8 @@
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="21"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="13"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
@@ -2363,10 +2524,10 @@
       <c r="O37" s="4"/>
     </row>
     <row r="38" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="19">
+      <c r="B38" s="11">
         <v>1040</v>
       </c>
       <c r="C38" s="4">
@@ -2377,8 +2538,8 @@
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="21"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="13"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
@@ -2386,10 +2547,10 @@
       <c r="O38" s="4"/>
     </row>
     <row r="39" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="19">
+      <c r="B39" s="11">
         <v>1100</v>
       </c>
       <c r="C39" s="4">
@@ -2400,8 +2561,8 @@
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="21"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="13"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -2409,10 +2570,10 @@
       <c r="O39" s="4"/>
     </row>
     <row r="40" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A40" s="18" t="s">
+      <c r="A40" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="19">
+      <c r="B40" s="11">
         <v>1100</v>
       </c>
       <c r="C40" s="4">
@@ -2424,7 +2585,7 @@
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
-      <c r="J40" s="23"/>
+      <c r="J40" s="15"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
@@ -2432,10 +2593,10 @@
       <c r="O40" s="4"/>
     </row>
     <row r="41" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="19">
+      <c r="B41" s="11">
         <v>1050</v>
       </c>
       <c r="C41" s="4">
@@ -2446,8 +2607,8 @@
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
-      <c r="I41" s="22"/>
-      <c r="J41" s="21"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="13"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
@@ -2455,10 +2616,10 @@
       <c r="O41" s="4"/>
     </row>
     <row r="42" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A42" s="18" t="s">
+      <c r="A42" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="19">
+      <c r="B42" s="11">
         <v>1130</v>
       </c>
       <c r="C42" s="4">
@@ -2469,8 +2630,8 @@
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
-      <c r="I42" s="22"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="13"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
@@ -2478,10 +2639,10 @@
       <c r="O42" s="4"/>
     </row>
     <row r="43" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A43" s="18" t="s">
+      <c r="A43" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="19">
+      <c r="B43" s="11">
         <v>1100</v>
       </c>
       <c r="C43" s="4">
@@ -2492,8 +2653,8 @@
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="21"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="13"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
@@ -2501,10 +2662,10 @@
       <c r="O43" s="4"/>
     </row>
     <row r="44" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A44" s="18" t="s">
+      <c r="A44" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B44" s="19">
+      <c r="B44" s="11">
         <v>1330</v>
       </c>
       <c r="C44" s="4">
@@ -2515,21 +2676,21 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-      <c r="I44" s="5" t="s">
+      <c r="I44" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="25"/>
+      <c r="J44" s="39"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5"/>
-      <c r="O44" s="26"/>
+      <c r="M44" s="30"/>
+      <c r="N44" s="30"/>
+      <c r="O44" s="17"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B45" s="19">
+      <c r="B45" s="11">
         <v>1200</v>
       </c>
       <c r="C45" s="4">
@@ -2540,19 +2701,19 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="5"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
+      <c r="K45" s="30"/>
+      <c r="L45" s="30"/>
+      <c r="M45" s="30"/>
+      <c r="N45" s="30"/>
+      <c r="O45" s="30"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A46" s="18" t="s">
+      <c r="A46" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B46" s="19">
+      <c r="B46" s="11">
         <v>1250</v>
       </c>
       <c r="C46" s="4">
@@ -2563,21 +2724,21 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="8" t="s">
+      <c r="I46" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="8"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="8"/>
-      <c r="N46" s="8"/>
-      <c r="O46" s="27"/>
+      <c r="J46" s="31"/>
+      <c r="K46" s="31"/>
+      <c r="L46" s="31"/>
+      <c r="M46" s="31"/>
+      <c r="N46" s="31"/>
+      <c r="O46" s="32"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B47" s="19">
+      <c r="B47" s="11">
         <v>1370</v>
       </c>
       <c r="C47" s="4">
@@ -2591,22 +2752,22 @@
       <c r="I47" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J47" s="23" t="s">
+      <c r="J47" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="5" t="s">
+      <c r="K47" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="28"/>
+      <c r="L47" s="30"/>
+      <c r="M47" s="30"/>
+      <c r="N47" s="30"/>
+      <c r="O47" s="33"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B48" s="19">
+      <c r="B48" s="11">
         <v>2780</v>
       </c>
       <c r="C48" s="4">
@@ -2620,18 +2781,18 @@
       <c r="I48" s="4">
         <v>1000</v>
       </c>
-      <c r="J48" s="23"/>
+      <c r="J48" s="15"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="28"/>
+      <c r="O48" s="33"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A49" s="18" t="s">
+      <c r="A49" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B49" s="19">
+      <c r="B49" s="11">
         <v>6540</v>
       </c>
       <c r="C49" s="4">
@@ -2645,12 +2806,12 @@
       <c r="I49" s="4">
         <v>500</v>
       </c>
-      <c r="J49" s="23"/>
+      <c r="J49" s="15"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="28"/>
+      <c r="O49" s="33"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1">
       <c r="A50" s="4" t="s">
@@ -2670,12 +2831,12 @@
       <c r="I50" s="4">
         <v>100</v>
       </c>
-      <c r="J50" s="23"/>
+      <c r="J50" s="15"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="28"/>
+      <c r="O50" s="33"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1">
       <c r="A51" s="4" t="s">
@@ -2695,12 +2856,12 @@
       <c r="I51" s="4">
         <v>50</v>
       </c>
-      <c r="J51" s="23"/>
+      <c r="J51" s="15"/>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="28"/>
+      <c r="O51" s="33"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1">
       <c r="A52" s="4" t="s">
@@ -2720,12 +2881,12 @@
       <c r="I52" s="4">
         <v>20</v>
       </c>
-      <c r="J52" s="23"/>
+      <c r="J52" s="15"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="28"/>
+      <c r="O52" s="33"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1">
       <c r="A53" s="4" t="s">
@@ -2745,12 +2906,12 @@
       <c r="I53" s="4">
         <v>10</v>
       </c>
-      <c r="J53" s="23"/>
+      <c r="J53" s="15"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="28"/>
+      <c r="O53" s="33"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1">
       <c r="A54" s="4" t="s">
@@ -2770,12 +2931,12 @@
       <c r="I54" s="4">
         <v>5</v>
       </c>
-      <c r="J54" s="23"/>
+      <c r="J54" s="15"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="28"/>
+      <c r="O54" s="33"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1">
       <c r="A55" s="4" t="s">
@@ -2795,26 +2956,26 @@
       <c r="I55" s="4">
         <v>2</v>
       </c>
-      <c r="J55" s="23"/>
+      <c r="J55" s="15"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="28"/>
+      <c r="O55" s="33"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A56" s="18" t="s">
+      <c r="A56" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B56" s="18">
+      <c r="B56" s="10">
         <v>9190</v>
       </c>
-      <c r="C56" s="18">
+      <c r="C56" s="10">
         <v>9990</v>
       </c>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4" t="s">
@@ -2825,111 +2986,103 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="29"/>
-    </row>
-    <row r="57" spans="1:15">
-      <c r="A57" s="30"/>
-      <c r="B57" s="31"/>
-      <c r="C57" s="32"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="30"/>
-      <c r="F57" s="30"/>
-      <c r="G57" s="30"/>
-      <c r="H57" s="30"/>
-      <c r="I57" s="30"/>
-      <c r="J57" s="33"/>
-      <c r="K57" s="32"/>
-      <c r="L57" s="32"/>
-      <c r="M57" s="34"/>
-      <c r="N57" s="34"/>
-      <c r="O57" s="34"/>
+      <c r="O56" s="34"/>
+    </row>
+    <row r="57" spans="1:15" ht="16.5" thickBot="1">
+      <c r="A57" s="18"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
+      <c r="J57" s="21"/>
+      <c r="K57" s="20"/>
+      <c r="L57" s="20"/>
+      <c r="M57" s="22"/>
+      <c r="N57" s="22"/>
+      <c r="O57" s="22"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="35" t="s">
+      <c r="A58" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="35"/>
-      <c r="C58" s="35"/>
-      <c r="D58" s="36"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="38" t="s">
+      <c r="B58" s="28"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="G58" s="38"/>
-      <c r="H58" s="38"/>
-      <c r="I58" s="38"/>
-      <c r="J58" s="38"/>
-      <c r="K58" s="38"/>
-      <c r="L58" s="36"/>
-      <c r="M58" s="37"/>
-      <c r="N58" s="39" t="s">
+      <c r="G58" s="46"/>
+      <c r="H58" s="46"/>
+      <c r="I58" s="46"/>
+      <c r="J58" s="46"/>
+      <c r="K58" s="47"/>
+      <c r="L58" s="23"/>
+      <c r="M58" s="24"/>
+      <c r="N58" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="39"/>
-    </row>
-    <row r="59" spans="1:15">
-      <c r="A59" s="40"/>
-      <c r="B59" s="40"/>
-      <c r="C59" s="40"/>
-      <c r="D59" s="32"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="38"/>
-      <c r="G59" s="38"/>
-      <c r="H59" s="38"/>
-      <c r="I59" s="38"/>
-      <c r="J59" s="38"/>
-      <c r="K59" s="38"/>
-      <c r="L59" s="32"/>
-      <c r="M59" s="30"/>
-      <c r="N59" s="40"/>
-      <c r="O59" s="40"/>
+      <c r="O58" s="29"/>
+    </row>
+    <row r="59" spans="1:15" ht="16.5" thickBot="1">
+      <c r="A59" s="38"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="38"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="48"/>
+      <c r="G59" s="49"/>
+      <c r="H59" s="49"/>
+      <c r="I59" s="49"/>
+      <c r="J59" s="49"/>
+      <c r="K59" s="50"/>
+      <c r="L59" s="20"/>
+      <c r="M59" s="18"/>
+      <c r="N59" s="38"/>
+      <c r="O59" s="38"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="40"/>
-      <c r="B60" s="40"/>
-      <c r="C60" s="40"/>
-      <c r="D60" s="32"/>
-      <c r="E60" s="30"/>
-      <c r="F60" s="30"/>
-      <c r="G60" s="30"/>
-      <c r="H60" s="30"/>
-      <c r="I60" s="30"/>
-      <c r="J60" s="33"/>
-      <c r="K60" s="32"/>
-      <c r="L60" s="32"/>
-      <c r="M60" s="30"/>
-      <c r="N60" s="40"/>
-      <c r="O60" s="40"/>
+      <c r="A60" s="38"/>
+      <c r="B60" s="38"/>
+      <c r="C60" s="38"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
+      <c r="J60" s="21"/>
+      <c r="K60" s="20"/>
+      <c r="L60" s="20"/>
+      <c r="M60" s="18"/>
+      <c r="N60" s="38"/>
+      <c r="O60" s="38"/>
     </row>
     <row r="61" spans="1:15">
-      <c r="A61" s="35" t="s">
+      <c r="A61" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="35"/>
-      <c r="C61" s="35"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="36"/>
-      <c r="F61" s="36"/>
-      <c r="G61" s="36"/>
-      <c r="H61" s="36"/>
-      <c r="I61" s="36"/>
-      <c r="J61" s="41"/>
-      <c r="K61" s="36"/>
-      <c r="L61" s="36"/>
-      <c r="M61" s="42"/>
-      <c r="N61" s="39"/>
-      <c r="O61" s="39"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="23"/>
+      <c r="F61" s="23"/>
+      <c r="G61" s="23"/>
+      <c r="H61" s="23"/>
+      <c r="I61" s="23"/>
+      <c r="J61" s="26"/>
+      <c r="K61" s="23"/>
+      <c r="L61" s="23"/>
+      <c r="M61" s="27"/>
+      <c r="N61" s="29"/>
+      <c r="O61" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="N61:O61"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="N58:O58"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="K1:O1"/>
     <mergeCell ref="A1:E1"/>
@@ -2942,6 +3095,14 @@
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="F58:K59"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="N58:O58"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.3" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -2952,82 +3113,98 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O64"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection sqref="A1:O61"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="3" max="4" width="8.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="1.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="3" customWidth="1"/>
+    <col min="11" max="12" width="7.140625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.75">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:15" ht="32.25" customHeight="1">
+      <c r="A1" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="9" t="s">
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-    </row>
-    <row r="2" spans="1:15" ht="15.75">
-      <c r="A2" s="12" t="s">
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.75">
-      <c r="A3" s="12" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+    </row>
+    <row r="3" spans="1:15" s="6" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A3" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-    </row>
-    <row r="4" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A4" s="7" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+    </row>
+    <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A4" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -3035,1573 +3212,1535 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="14" t="s">
+      <c r="L4" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="H5" s="16"/>
-      <c r="I5" s="15" t="s">
+      <c r="H5" s="8"/>
+      <c r="I5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="L5" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="M5" s="16" t="s">
+      <c r="M5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="16" t="s">
+      <c r="N5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="16" t="s">
+      <c r="O5" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75">
-      <c r="A6" s="18" t="s">
+    <row r="6" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A6" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="11">
         <v>800</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="5">
         <v>875</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="20" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="J6" s="21">
+      <c r="J6" s="13">
         <v>5750</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="5">
         <v>6190</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-    </row>
-    <row r="7" spans="1:15" ht="15.75">
-      <c r="A7" s="18" t="s">
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A7" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="11">
         <v>780</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="5">
         <v>840</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="22" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="J7" s="23">
+      <c r="J7" s="15">
         <v>4640</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="5">
         <v>4990</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-    </row>
-    <row r="8" spans="1:15" ht="15.75">
-      <c r="A8" s="18" t="s">
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A8" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="11">
         <v>865</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="5">
         <v>925</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="18" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="10">
         <v>5650</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="5">
         <v>6150</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-    </row>
-    <row r="9" spans="1:15" ht="15.75">
-      <c r="A9" s="18" t="s">
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="11">
         <v>810</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="5">
         <v>880</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="18" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="13">
         <v>5020</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="5">
         <v>5390</v>
       </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-    </row>
-    <row r="10" spans="1:15" ht="15.75">
-      <c r="A10" s="18" t="s">
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A10" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="11">
         <v>800</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="5">
         <v>870</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="22" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="13">
         <v>5280</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="5">
         <v>5690</v>
       </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-    </row>
-    <row r="11" spans="1:15" ht="15.75">
-      <c r="A11" s="18" t="s">
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="11">
         <v>795</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="5">
         <v>865</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="22" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="13">
         <v>4820</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="5">
         <v>5190</v>
       </c>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-    </row>
-    <row r="12" spans="1:15" ht="15.75">
-      <c r="A12" s="18" t="s">
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="11">
         <v>790</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="5">
         <v>860</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="18" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="J12" s="21">
+      <c r="J12" s="13">
         <v>5100</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="5">
         <v>5490</v>
       </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-    </row>
-    <row r="13" spans="1:15" ht="15.75">
-      <c r="A13" s="18" t="s">
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A13" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="11">
         <v>800</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="5">
         <v>860</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="20" t="s">
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="21">
+      <c r="J13" s="13">
         <v>5560</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="5">
         <v>5990</v>
       </c>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-    </row>
-    <row r="14" spans="1:15" ht="15.75">
-      <c r="A14" s="18" t="s">
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+    </row>
+    <row r="14" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="11">
         <v>970</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="5">
         <v>1060</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="18" t="s">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="J14" s="21">
+      <c r="J14" s="13">
         <v>6090</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="5">
         <v>6590</v>
       </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-    </row>
-    <row r="15" spans="1:15" ht="15.75">
-      <c r="A15" s="18" t="s">
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+    </row>
+    <row r="15" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A15" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="11">
         <v>900</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="5">
         <v>975</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="20" t="s">
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="J15" s="21">
+      <c r="J15" s="13">
         <v>5390</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="5">
         <v>5790</v>
       </c>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-    </row>
-    <row r="16" spans="1:15" ht="15.75">
-      <c r="A16" s="18" t="s">
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+    </row>
+    <row r="16" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A16" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="11">
         <v>915</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="5">
         <v>990</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="20" t="s">
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="J16" s="21">
+      <c r="J16" s="13">
         <v>3630</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="5">
         <v>3890</v>
       </c>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-    </row>
-    <row r="17" spans="1:15" ht="15.75">
-      <c r="A17" s="18" t="s">
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+    </row>
+    <row r="17" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A17" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="11">
         <v>910</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="5">
         <v>980</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="18" t="s">
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J17" s="21">
+      <c r="J17" s="13">
         <v>3560</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="5">
         <v>3840</v>
       </c>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-    </row>
-    <row r="18" spans="1:15" ht="15.75">
-      <c r="A18" s="18" t="s">
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+    </row>
+    <row r="18" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A18" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="19">
+      <c r="B18" s="11">
         <v>890</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="5">
         <v>970</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="18" t="s">
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="J18" s="21">
+      <c r="J18" s="13">
         <v>3340</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18" s="5">
         <v>3590</v>
       </c>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-    </row>
-    <row r="19" spans="1:15" ht="15.75">
-      <c r="A19" s="18" t="s">
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+    </row>
+    <row r="19" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A19" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="19">
+      <c r="B19" s="11">
         <v>920</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="5">
         <v>999</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="20" t="s">
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="J19" s="21">
+      <c r="J19" s="13">
         <v>5390</v>
       </c>
-      <c r="K19" s="4">
+      <c r="K19" s="5">
         <v>5790</v>
       </c>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-    </row>
-    <row r="20" spans="1:15" ht="15.75">
-      <c r="A20" s="18" t="s">
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+    </row>
+    <row r="20" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A20" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="19">
+      <c r="B20" s="11">
         <v>880</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="5">
         <v>950</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="18" t="s">
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="J20" s="21">
+      <c r="J20" s="13">
         <v>4500</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="5">
         <v>4790</v>
       </c>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-    </row>
-    <row r="21" spans="1:15" ht="15.75">
-      <c r="A21" s="18" t="s">
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+    </row>
+    <row r="21" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A21" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="19">
+      <c r="B21" s="11">
         <v>1000</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="5">
         <v>1090</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="18" t="s">
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="J21" s="21">
+      <c r="J21" s="13">
         <v>4970</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="5">
         <v>5290</v>
       </c>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-    </row>
-    <row r="22" spans="1:15" ht="15.75">
-      <c r="A22" s="18" t="s">
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A22" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="19">
+      <c r="B22" s="11">
         <v>995</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="5">
         <v>1075</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="18" t="s">
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="J22" s="21">
+      <c r="J22" s="13">
         <v>4015</v>
       </c>
-      <c r="K22" s="4">
+      <c r="K22" s="5">
         <v>4390</v>
       </c>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-    </row>
-    <row r="23" spans="1:15" ht="15.75">
-      <c r="A23" s="18" t="s">
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+    </row>
+    <row r="23" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A23" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="19">
+      <c r="B23" s="11">
         <v>1000</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="5">
         <v>1090</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="18" t="s">
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="21">
+      <c r="J23" s="13">
         <v>3710</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23" s="5">
         <v>3990</v>
       </c>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-    </row>
-    <row r="24" spans="1:15" ht="15.75">
-      <c r="A24" s="18" t="s">
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A24" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B24" s="11">
         <v>960</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="5">
         <v>1040</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="18" t="s">
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="J24" s="21">
+      <c r="J24" s="13">
         <v>3620</v>
       </c>
-      <c r="K24" s="4">
+      <c r="K24" s="5">
         <v>3890</v>
       </c>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-    </row>
-    <row r="25" spans="1:15" ht="15.75">
-      <c r="A25" s="18" t="s">
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A25" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="11">
         <v>1040</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="5">
         <v>1120</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="18" t="s">
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J25" s="21">
+      <c r="J25" s="13">
         <v>4620</v>
       </c>
-      <c r="K25" s="4">
+      <c r="K25" s="5">
         <v>4999</v>
       </c>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-    </row>
-    <row r="26" spans="1:15" ht="15.75">
-      <c r="A26" s="18" t="s">
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+    </row>
+    <row r="26" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A26" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B26" s="19">
+      <c r="B26" s="11">
         <v>930</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="5">
         <v>999</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="18" t="s">
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="J26" s="21">
+      <c r="J26" s="13">
         <v>4520</v>
       </c>
-      <c r="K26" s="4">
+      <c r="K26" s="5">
         <v>4899</v>
       </c>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-    </row>
-    <row r="27" spans="1:15" ht="15.75">
-      <c r="A27" s="18" t="s">
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A27" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="11">
         <v>1290</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="5">
         <v>1390</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="18" t="s">
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="J27" s="21">
+      <c r="J27" s="13">
         <v>4080</v>
       </c>
-      <c r="K27" s="4">
+      <c r="K27" s="5">
         <v>4390</v>
       </c>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-    </row>
-    <row r="28" spans="1:15" ht="15.75">
-      <c r="A28" s="18" t="s">
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+    </row>
+    <row r="28" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A28" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B28" s="19">
+      <c r="B28" s="11">
         <v>1190</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="5">
         <v>1290</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="22" t="s">
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="J28" s="21">
+      <c r="J28" s="13">
         <v>4220</v>
       </c>
-      <c r="K28" s="4">
+      <c r="K28" s="5">
         <v>4540</v>
       </c>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-    </row>
-    <row r="29" spans="1:15" ht="15.75">
-      <c r="A29" s="18" t="s">
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+    </row>
+    <row r="29" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A29" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="19">
+      <c r="B29" s="11">
         <v>1270</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="5">
         <v>1370</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="22" t="s">
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="J29" s="21">
+      <c r="J29" s="13">
         <v>12240</v>
       </c>
-      <c r="K29" s="4">
+      <c r="K29" s="5">
         <v>12990</v>
       </c>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-    </row>
-    <row r="30" spans="1:15" ht="15.75">
-      <c r="A30" s="18" t="s">
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+    </row>
+    <row r="30" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A30" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="19">
+      <c r="B30" s="11">
         <v>1170</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="5">
         <v>1270</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="18" t="s">
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="J30" s="23">
+      <c r="J30" s="15">
         <v>12090</v>
       </c>
-      <c r="K30" s="4">
+      <c r="K30" s="5">
         <v>12990</v>
       </c>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-    </row>
-    <row r="31" spans="1:15" ht="15.75">
-      <c r="A31" s="18" t="s">
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+    </row>
+    <row r="31" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A31" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="19">
+      <c r="B31" s="11">
         <v>1190</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="5">
         <v>1290</v>
       </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="20" t="s">
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="J31" s="23">
+      <c r="J31" s="15">
         <v>10840</v>
       </c>
-      <c r="K31" s="4">
+      <c r="K31" s="5">
         <v>11990</v>
       </c>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-    </row>
-    <row r="32" spans="1:15" ht="15.75">
-      <c r="A32" s="18" t="s">
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+    </row>
+    <row r="32" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A32" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B32" s="19">
+      <c r="B32" s="11">
         <v>1225</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="5">
         <v>1325</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="20" t="s">
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="J32" s="23">
+      <c r="J32" s="15">
         <v>12490</v>
       </c>
-      <c r="K32" s="4">
+      <c r="K32" s="5">
         <v>13490</v>
       </c>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-    </row>
-    <row r="33" spans="1:15" ht="15.75">
-      <c r="A33" s="18" t="s">
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+    </row>
+    <row r="33" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A33" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="19">
+      <c r="B33" s="11">
         <v>1220</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="5">
         <v>1320</v>
       </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="20" t="s">
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="J33" s="21">
+      <c r="J33" s="13">
         <v>8820</v>
       </c>
-      <c r="K33" s="4">
+      <c r="K33" s="5">
         <v>9490</v>
       </c>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-    </row>
-    <row r="34" spans="1:15" ht="15.75">
-      <c r="A34" s="18" t="s">
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+    </row>
+    <row r="34" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A34" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="19">
+      <c r="B34" s="11">
         <v>1080</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="5">
         <v>1160</v>
       </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="23"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-    </row>
-    <row r="35" spans="1:15" ht="15.75">
-      <c r="A35" s="18" t="s">
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+    </row>
+    <row r="35" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A35" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="19">
+      <c r="B35" s="11">
         <v>1100</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="5">
         <v>1199</v>
       </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-    </row>
-    <row r="36" spans="1:15" ht="15.75">
-      <c r="A36" s="18" t="s">
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+    </row>
+    <row r="36" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A36" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="24">
+      <c r="B36" s="16">
         <v>1200</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="5">
         <v>1290</v>
       </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-    </row>
-    <row r="37" spans="1:15" ht="15.75">
-      <c r="A37" s="18" t="s">
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+    </row>
+    <row r="37" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A37" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="19">
+      <c r="B37" s="11">
         <v>1120</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="5">
         <v>1220</v>
       </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-    </row>
-    <row r="38" spans="1:15" ht="15.75">
-      <c r="A38" s="18" t="s">
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+    </row>
+    <row r="38" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A38" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="19">
+      <c r="B38" s="11">
         <v>1040</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="5">
         <v>1130</v>
       </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-    </row>
-    <row r="39" spans="1:15" ht="15.75">
-      <c r="A39" s="18" t="s">
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+    </row>
+    <row r="39" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A39" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="19">
+      <c r="B39" s="11">
         <v>1100</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="5">
         <v>1199</v>
       </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-    </row>
-    <row r="40" spans="1:15" ht="15.75">
-      <c r="A40" s="18" t="s">
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+    </row>
+    <row r="40" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A40" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="19">
+      <c r="B40" s="11">
         <v>1100</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="5">
         <v>1199</v>
       </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="23"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
-    </row>
-    <row r="41" spans="1:15" ht="15.75">
-      <c r="A41" s="18" t="s">
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+    </row>
+    <row r="41" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A41" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="19">
+      <c r="B41" s="11">
         <v>1050</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="5">
         <v>1130</v>
       </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="22"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-    </row>
-    <row r="42" spans="1:15" ht="15.75">
-      <c r="A42" s="18" t="s">
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+    </row>
+    <row r="42" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A42" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="19">
+      <c r="B42" s="11">
         <v>1130</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="5">
         <v>1230</v>
       </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="22"/>
-      <c r="J42" s="21"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
-      <c r="N42" s="4"/>
-      <c r="O42" s="4"/>
-    </row>
-    <row r="43" spans="1:15" ht="15.75">
-      <c r="A43" s="18" t="s">
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+    </row>
+    <row r="43" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A43" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="19">
+      <c r="B43" s="11">
         <v>1100</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="5">
         <v>1190</v>
       </c>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
-    </row>
-    <row r="44" spans="1:15" ht="15.75">
-      <c r="A44" s="18" t="s">
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+    </row>
+    <row r="44" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A44" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B44" s="19">
+      <c r="B44" s="11">
         <v>1330</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44" s="5">
         <v>1450</v>
       </c>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="5" t="s">
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="25"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5"/>
-      <c r="O44" s="26"/>
-    </row>
-    <row r="45" spans="1:15" ht="15.75">
-      <c r="A45" s="18" t="s">
+      <c r="J44" s="39"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="30"/>
+      <c r="N44" s="30"/>
+      <c r="O44" s="17"/>
+    </row>
+    <row r="45" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A45" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B45" s="19">
+      <c r="B45" s="11">
         <v>1200</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C45" s="5">
         <v>1299</v>
       </c>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="5"/>
-    </row>
-    <row r="46" spans="1:15" ht="15.75">
-      <c r="A46" s="18" t="s">
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
+      <c r="K45" s="30"/>
+      <c r="L45" s="30"/>
+      <c r="M45" s="30"/>
+      <c r="N45" s="30"/>
+      <c r="O45" s="30"/>
+    </row>
+    <row r="46" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A46" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B46" s="19">
+      <c r="B46" s="11">
         <v>1250</v>
       </c>
-      <c r="C46" s="4">
+      <c r="C46" s="5">
         <v>1350</v>
       </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="8" t="s">
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="8"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="8"/>
-      <c r="N46" s="8"/>
-      <c r="O46" s="27"/>
-    </row>
-    <row r="47" spans="1:15" ht="15.75">
-      <c r="A47" s="18" t="s">
+      <c r="J46" s="31"/>
+      <c r="K46" s="31"/>
+      <c r="L46" s="31"/>
+      <c r="M46" s="31"/>
+      <c r="N46" s="31"/>
+      <c r="O46" s="32"/>
+    </row>
+    <row r="47" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A47" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B47" s="19">
+      <c r="B47" s="11">
         <v>1370</v>
       </c>
-      <c r="C47" s="4">
+      <c r="C47" s="5">
         <v>1490</v>
       </c>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4" t="s">
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="J47" s="23" t="s">
+      <c r="J47" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="5" t="s">
+      <c r="K47" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="28"/>
-    </row>
-    <row r="48" spans="1:15" ht="15.75">
-      <c r="A48" s="18" t="s">
+      <c r="L47" s="30"/>
+      <c r="M47" s="30"/>
+      <c r="N47" s="30"/>
+      <c r="O47" s="33"/>
+    </row>
+    <row r="48" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A48" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B48" s="19">
+      <c r="B48" s="11">
         <v>2780</v>
       </c>
-      <c r="C48" s="4">
+      <c r="C48" s="5">
         <v>2990</v>
       </c>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4">
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5">
         <v>1000</v>
       </c>
-      <c r="J48" s="23"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
-      <c r="O48" s="28"/>
-    </row>
-    <row r="49" spans="1:15" ht="15.75">
-      <c r="A49" s="18" t="s">
+      <c r="J48" s="15"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="33"/>
+    </row>
+    <row r="49" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A49" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B49" s="19">
+      <c r="B49" s="11">
         <v>6540</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C49" s="5">
         <v>6990</v>
       </c>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4">
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5">
         <v>500</v>
       </c>
-      <c r="J49" s="23"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="28"/>
-    </row>
-    <row r="50" spans="1:15" ht="15.75">
-      <c r="A50" s="4" t="s">
+      <c r="J49" s="15"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="5"/>
+      <c r="O49" s="33"/>
+    </row>
+    <row r="50" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A50" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B50" s="5">
         <v>5290</v>
       </c>
-      <c r="C50" s="4">
+      <c r="C50" s="5">
         <v>5690</v>
       </c>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4">
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5">
         <v>100</v>
       </c>
-      <c r="J50" s="23"/>
-      <c r="K50" s="4"/>
-      <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
-      <c r="N50" s="4"/>
-      <c r="O50" s="28"/>
-    </row>
-    <row r="51" spans="1:15" ht="15.75">
-      <c r="A51" s="4" t="s">
+      <c r="J50" s="15"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="5"/>
+      <c r="O50" s="33"/>
+    </row>
+    <row r="51" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A51" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B51" s="4">
+      <c r="B51" s="5">
         <v>5470</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C51" s="5">
         <v>5890</v>
       </c>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
-      <c r="I51" s="4">
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5">
         <v>50</v>
       </c>
-      <c r="J51" s="23"/>
-      <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
-      <c r="N51" s="4"/>
-      <c r="O51" s="28"/>
-    </row>
-    <row r="52" spans="1:15" ht="15.75">
-      <c r="A52" s="4" t="s">
+      <c r="J51" s="15"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5"/>
+      <c r="O51" s="33"/>
+    </row>
+    <row r="52" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A52" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B52" s="4">
+      <c r="B52" s="5">
         <v>5750</v>
       </c>
-      <c r="C52" s="4">
+      <c r="C52" s="5">
         <v>6190</v>
       </c>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
-      <c r="I52" s="4">
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5">
         <v>20</v>
       </c>
-      <c r="J52" s="23"/>
-      <c r="K52" s="4"/>
-      <c r="L52" s="4"/>
-      <c r="M52" s="4"/>
-      <c r="N52" s="4"/>
-      <c r="O52" s="28"/>
-    </row>
-    <row r="53" spans="1:15" ht="15.75">
-      <c r="A53" s="4" t="s">
+      <c r="J52" s="15"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5"/>
+      <c r="N52" s="5"/>
+      <c r="O52" s="33"/>
+    </row>
+    <row r="53" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A53" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="4">
+      <c r="B53" s="5">
         <v>5940</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C53" s="5">
         <v>6390</v>
       </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4">
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5">
         <v>10</v>
       </c>
-      <c r="J53" s="23"/>
-      <c r="K53" s="4"/>
-      <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
-      <c r="N53" s="4"/>
-      <c r="O53" s="28"/>
-    </row>
-    <row r="54" spans="1:15" ht="15.75">
-      <c r="A54" s="4" t="s">
+      <c r="J53" s="15"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="33"/>
+    </row>
+    <row r="54" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A54" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B54" s="4">
+      <c r="B54" s="5">
         <v>6530</v>
       </c>
-      <c r="C54" s="4">
+      <c r="C54" s="5">
         <v>6990</v>
       </c>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4">
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5">
         <v>5</v>
       </c>
-      <c r="J54" s="23"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
-      <c r="N54" s="4"/>
-      <c r="O54" s="28"/>
-    </row>
-    <row r="55" spans="1:15" ht="15.75">
-      <c r="A55" s="4" t="s">
+      <c r="J54" s="15"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="33"/>
+    </row>
+    <row r="55" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A55" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B55" s="4">
+      <c r="B55" s="5">
         <v>8340</v>
       </c>
-      <c r="C55" s="4">
+      <c r="C55" s="5">
         <v>8990</v>
       </c>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4">
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5">
         <v>2</v>
       </c>
-      <c r="J55" s="23"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
-      <c r="N55" s="4"/>
-      <c r="O55" s="28"/>
-    </row>
-    <row r="56" spans="1:15" ht="15.75">
-      <c r="A56" s="18" t="s">
+      <c r="J55" s="15"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
+      <c r="O55" s="33"/>
+    </row>
+    <row r="56" spans="1:15" ht="15.95" customHeight="1">
+      <c r="A56" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B56" s="18">
+      <c r="B56" s="10">
         <v>9190</v>
       </c>
-      <c r="C56" s="18">
+      <c r="C56" s="10">
         <v>9990</v>
       </c>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4" t="s">
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-      <c r="M56" s="4"/>
-      <c r="N56" s="4"/>
-      <c r="O56" s="29"/>
-    </row>
-    <row r="57" spans="1:15" ht="15.75">
-      <c r="A57" s="30"/>
-      <c r="B57" s="31"/>
-      <c r="C57" s="32"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="30"/>
-      <c r="F57" s="30"/>
-      <c r="G57" s="30"/>
-      <c r="H57" s="30"/>
-      <c r="I57" s="30"/>
-      <c r="J57" s="33"/>
-      <c r="K57" s="32"/>
-      <c r="L57" s="32"/>
-      <c r="M57" s="34"/>
-      <c r="N57" s="34"/>
-      <c r="O57" s="34"/>
-    </row>
-    <row r="58" spans="1:15" ht="15" customHeight="1">
-      <c r="A58" s="35" t="s">
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="5"/>
+      <c r="O56" s="34"/>
+    </row>
+    <row r="57" spans="1:15">
+      <c r="A57" s="18"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="25"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
+      <c r="J57" s="21"/>
+      <c r="K57" s="25"/>
+      <c r="L57" s="25"/>
+      <c r="M57" s="22"/>
+      <c r="N57" s="22"/>
+      <c r="O57" s="22"/>
+    </row>
+    <row r="58" spans="1:15">
+      <c r="A58" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="35"/>
-      <c r="C58" s="35"/>
-      <c r="D58" s="36"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="38" t="s">
+      <c r="B58" s="28"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="G58" s="38"/>
-      <c r="H58" s="38"/>
-      <c r="I58" s="38"/>
-      <c r="J58" s="38"/>
-      <c r="K58" s="38"/>
-      <c r="L58" s="36"/>
-      <c r="M58" s="37"/>
-      <c r="N58" s="39" t="s">
+      <c r="G58" s="44"/>
+      <c r="H58" s="44"/>
+      <c r="I58" s="44"/>
+      <c r="J58" s="44"/>
+      <c r="K58" s="44"/>
+      <c r="L58" s="23"/>
+      <c r="M58" s="24"/>
+      <c r="N58" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="39"/>
-    </row>
-    <row r="59" spans="1:15" ht="15" customHeight="1">
-      <c r="A59" s="40"/>
-      <c r="B59" s="40"/>
-      <c r="C59" s="40"/>
-      <c r="D59" s="32"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="38"/>
-      <c r="G59" s="38"/>
-      <c r="H59" s="38"/>
-      <c r="I59" s="38"/>
-      <c r="J59" s="38"/>
-      <c r="K59" s="38"/>
-      <c r="L59" s="32"/>
-      <c r="M59" s="30"/>
-      <c r="N59" s="40"/>
-      <c r="O59" s="40"/>
-    </row>
-    <row r="60" spans="1:15" ht="15.75">
-      <c r="A60" s="40"/>
-      <c r="B60" s="40"/>
-      <c r="C60" s="40"/>
-      <c r="D60" s="32"/>
-      <c r="E60" s="30"/>
-      <c r="F60" s="30"/>
-      <c r="G60" s="30"/>
-      <c r="H60" s="30"/>
-      <c r="I60" s="30"/>
-      <c r="J60" s="33"/>
-      <c r="K60" s="32"/>
-      <c r="L60" s="32"/>
-      <c r="M60" s="30"/>
-      <c r="N60" s="40"/>
-      <c r="O60" s="40"/>
-    </row>
-    <row r="61" spans="1:15" ht="15.75">
-      <c r="A61" s="35" t="s">
+      <c r="O58" s="29"/>
+    </row>
+    <row r="59" spans="1:15">
+      <c r="A59" s="38"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="38"/>
+      <c r="D59" s="25"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="44"/>
+      <c r="G59" s="44"/>
+      <c r="H59" s="44"/>
+      <c r="I59" s="44"/>
+      <c r="J59" s="44"/>
+      <c r="K59" s="44"/>
+      <c r="L59" s="25"/>
+      <c r="M59" s="18"/>
+      <c r="N59" s="38"/>
+      <c r="O59" s="38"/>
+    </row>
+    <row r="60" spans="1:15">
+      <c r="A60" s="38"/>
+      <c r="B60" s="38"/>
+      <c r="C60" s="38"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
+      <c r="J60" s="21"/>
+      <c r="K60" s="25"/>
+      <c r="L60" s="25"/>
+      <c r="M60" s="18"/>
+      <c r="N60" s="38"/>
+      <c r="O60" s="38"/>
+    </row>
+    <row r="61" spans="1:15">
+      <c r="A61" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="35"/>
-      <c r="C61" s="35"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="36"/>
-      <c r="F61" s="36"/>
-      <c r="G61" s="36"/>
-      <c r="H61" s="36"/>
-      <c r="I61" s="36"/>
-      <c r="J61" s="41"/>
-      <c r="K61" s="36"/>
-      <c r="L61" s="36"/>
-      <c r="M61" s="42"/>
-      <c r="N61" s="39"/>
-      <c r="O61" s="39"/>
-    </row>
-    <row r="62" spans="1:15" ht="15.75">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
-      <c r="J62" s="3"/>
-      <c r="K62" s="3"/>
-      <c r="L62" s="3"/>
-      <c r="M62" s="3"/>
-      <c r="N62" s="3"/>
-      <c r="O62" s="3"/>
-    </row>
-    <row r="63" spans="1:15" ht="15.75">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-      <c r="I63" s="3"/>
-      <c r="J63" s="3"/>
-      <c r="K63" s="3"/>
-      <c r="L63" s="3"/>
-      <c r="M63" s="3"/>
-      <c r="N63" s="3"/>
-      <c r="O63" s="3"/>
-    </row>
-    <row r="64" spans="1:15" ht="15.75">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-      <c r="I64" s="3"/>
-      <c r="J64" s="3"/>
-      <c r="K64" s="3"/>
-      <c r="L64" s="3"/>
-      <c r="M64" s="3"/>
-      <c r="N64" s="3"/>
-      <c r="O64" s="3"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="23"/>
+      <c r="F61" s="23"/>
+      <c r="G61" s="23"/>
+      <c r="H61" s="23"/>
+      <c r="I61" s="23"/>
+      <c r="J61" s="26"/>
+      <c r="K61" s="23"/>
+      <c r="L61" s="23"/>
+      <c r="M61" s="27"/>
+      <c r="N61" s="29"/>
+      <c r="O61" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="N58:O58"/>
+    <mergeCell ref="A59:C60"/>
+    <mergeCell ref="N59:O60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="F58:K59"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="A1:E1"/>
@@ -4609,19 +4748,6 @@
     <mergeCell ref="K1:O1"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A3:O3"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="N58:O58"/>
-    <mergeCell ref="A59:C60"/>
-    <mergeCell ref="N59:O60"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="N61:O61"/>
-    <mergeCell ref="F58:K59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
21.07.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/July/Others/Allocation Sheet.xlsx
+++ b/July/Others/Allocation Sheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="107">
   <si>
     <t>BL60</t>
   </si>
@@ -323,10 +323,19 @@
     <t>DSR NAME:   Md Shohel Rana</t>
   </si>
   <si>
-    <t>Robiul: 01751-312831</t>
-  </si>
-  <si>
-    <t>DSR NAME:   Md Robiul Islam</t>
+    <t>D37</t>
+  </si>
+  <si>
+    <t>BL97</t>
+  </si>
+  <si>
+    <t>Distributor: Symphony (Mobile Handset) Edison-Group</t>
+  </si>
+  <si>
+    <t>Madrasha Market , Bagha Bazar , Bagha , Rajshahi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Total Qnt:</t>
   </si>
 </sst>
 </file>
@@ -336,7 +345,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -410,6 +419,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -580,7 +603,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -653,15 +676,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -674,53 +724,47 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -739,14 +783,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>29158</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>9719</xdr:rowOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>162121</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>38878</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>9720</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -754,13 +798,14 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="29158" y="12639869"/>
-          <a:ext cx="1495620" cy="1"/>
+        <a:xfrm>
+          <a:off x="29158" y="12744646"/>
+          <a:ext cx="1761542" cy="9329"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln w="12700"/>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="1">
@@ -781,16 +826,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>466726</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>194388</xdr:rowOff>
+      <xdr:rowOff>175338</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>9719</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>895544</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>194390</xdr:rowOff>
+      <xdr:rowOff>175340</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -799,12 +844,13 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5753101" y="12614988"/>
-          <a:ext cx="1514668" cy="2"/>
+          <a:off x="7067551" y="12757863"/>
+          <a:ext cx="1524193" cy="2"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln w="12700"/>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="1">
@@ -1470,8 +1516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O64" sqref="A1:O64"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="R66" sqref="R66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1493,73 +1539,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="35" t="s">
+      <c r="A1" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="36" t="s">
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
+      <c r="A2" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
     </row>
     <row r="3" spans="1:15" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
+      <c r="A3" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1567,59 +1613,59 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="42" t="s">
-        <v>103</v>
-      </c>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
+      <c r="L4" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="7" t="s">
+      <c r="H5" s="49"/>
+      <c r="I5" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="L5" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="N5" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="O5" s="49" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.95" customHeight="1">
+    <row r="6" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>44</v>
       </c>
@@ -1635,20 +1681,20 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="12" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="J6" s="13">
-        <v>5750</v>
+        <v>9190</v>
       </c>
       <c r="K6" s="4">
-        <v>6190</v>
+        <v>9990</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="1:15" ht="15.95" customHeight="1">
+    <row r="7" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>95</v>
       </c>
@@ -1664,20 +1710,20 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="14" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J7" s="15">
-        <v>4640</v>
+        <v>5750</v>
       </c>
       <c r="K7" s="4">
-        <v>4990</v>
+        <v>6190</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
     </row>
-    <row r="8" spans="1:15" ht="15.95" customHeight="1">
+    <row r="8" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="10" t="s">
         <v>97</v>
       </c>
@@ -1693,20 +1739,20 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="10" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="J8" s="10">
-        <v>5650</v>
+        <v>4640</v>
       </c>
       <c r="K8" s="4">
-        <v>6150</v>
+        <v>4990</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
     </row>
-    <row r="9" spans="1:15" ht="15.95" customHeight="1">
+    <row r="9" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>39</v>
       </c>
@@ -1722,20 +1768,20 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="10" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="J9" s="13">
-        <v>5020</v>
+        <v>5650</v>
       </c>
       <c r="K9" s="4">
-        <v>5390</v>
+        <v>6150</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
     </row>
-    <row r="10" spans="1:15" ht="15.95" customHeight="1">
+    <row r="10" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>51</v>
       </c>
@@ -1751,20 +1797,20 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="14" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="J10" s="13">
-        <v>5280</v>
+        <v>5020</v>
       </c>
       <c r="K10" s="4">
-        <v>5690</v>
+        <v>5390</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
     </row>
-    <row r="11" spans="1:15" ht="15.95" customHeight="1">
+    <row r="11" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="10" t="s">
         <v>17</v>
       </c>
@@ -1780,20 +1826,20 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="14" t="s">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="J11" s="13">
-        <v>4820</v>
+        <v>5280</v>
       </c>
       <c r="K11" s="4">
-        <v>5190</v>
+        <v>5690</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
     </row>
-    <row r="12" spans="1:15" ht="15.95" customHeight="1">
+    <row r="12" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="10" t="s">
         <v>26</v>
       </c>
@@ -1809,20 +1855,20 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="10" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="J12" s="13">
-        <v>5100</v>
+        <v>4820</v>
       </c>
       <c r="K12" s="4">
-        <v>5490</v>
+        <v>5190</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
     </row>
-    <row r="13" spans="1:15" ht="15.95" customHeight="1">
+    <row r="13" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="10" t="s">
         <v>94</v>
       </c>
@@ -1838,20 +1884,20 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="12" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="J13" s="13">
-        <v>5560</v>
+        <v>5100</v>
       </c>
       <c r="K13" s="4">
-        <v>5990</v>
+        <v>5490</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
     </row>
-    <row r="14" spans="1:15" ht="15.95" customHeight="1">
+    <row r="14" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>18</v>
       </c>
@@ -1867,20 +1913,20 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="10" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="J14" s="13">
-        <v>6090</v>
+        <v>5560</v>
       </c>
       <c r="K14" s="4">
-        <v>6590</v>
+        <v>5990</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
     </row>
-    <row r="15" spans="1:15" ht="15.95" customHeight="1">
+    <row r="15" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="10" t="s">
         <v>73</v>
       </c>
@@ -1896,20 +1942,20 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="12" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="J15" s="13">
-        <v>5390</v>
+        <v>6090</v>
       </c>
       <c r="K15" s="4">
-        <v>5790</v>
+        <v>6590</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
     </row>
-    <row r="16" spans="1:15" ht="15.95" customHeight="1">
+    <row r="16" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="10" t="s">
         <v>0</v>
       </c>
@@ -1925,20 +1971,20 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="12" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="J16" s="13">
-        <v>3630</v>
+        <v>5390</v>
       </c>
       <c r="K16" s="4">
-        <v>3890</v>
+        <v>5790</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
     </row>
-    <row r="17" spans="1:15" ht="15.95" customHeight="1">
+    <row r="17" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>52</v>
       </c>
@@ -1954,20 +2000,20 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="10" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="J17" s="13">
-        <v>3560</v>
+        <v>3630</v>
       </c>
       <c r="K17" s="4">
-        <v>3840</v>
+        <v>3890</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
     </row>
-    <row r="18" spans="1:15" ht="15.95" customHeight="1">
+    <row r="18" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A18" s="10" t="s">
         <v>16</v>
       </c>
@@ -1983,20 +2029,20 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="10" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="J18" s="13">
-        <v>3340</v>
+        <v>3560</v>
       </c>
       <c r="K18" s="4">
-        <v>3590</v>
+        <v>3840</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
     </row>
-    <row r="19" spans="1:15" ht="15.95" customHeight="1">
+    <row r="19" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="10" t="s">
         <v>2</v>
       </c>
@@ -2012,20 +2058,20 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="12" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="J19" s="13">
-        <v>5390</v>
+        <v>3340</v>
       </c>
       <c r="K19" s="4">
-        <v>5790</v>
+        <v>3590</v>
       </c>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
     </row>
-    <row r="20" spans="1:15" ht="15.95" customHeight="1">
+    <row r="20" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="10" t="s">
         <v>35</v>
       </c>
@@ -2041,28 +2087,28 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="10" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="J20" s="13">
-        <v>4500</v>
+        <v>5390</v>
       </c>
       <c r="K20" s="4">
-        <v>4790</v>
+        <v>5790</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
     </row>
-    <row r="21" spans="1:15" ht="15.95" customHeight="1">
+    <row r="21" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="B21" s="11">
-        <v>1000</v>
+        <v>845</v>
       </c>
       <c r="C21" s="4">
-        <v>1090</v>
+        <v>910</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -2070,28 +2116,28 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="10" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="J21" s="13">
-        <v>4970</v>
+        <v>4500</v>
       </c>
       <c r="K21" s="4">
-        <v>5290</v>
+        <v>4790</v>
       </c>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
     </row>
-    <row r="22" spans="1:15" ht="15.95" customHeight="1">
+    <row r="22" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="10" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B22" s="11">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="C22" s="4">
-        <v>1075</v>
+        <v>1090</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -2099,28 +2145,28 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="10" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="J22" s="13">
-        <v>4015</v>
+        <v>4970</v>
       </c>
       <c r="K22" s="4">
-        <v>4390</v>
+        <v>5290</v>
       </c>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
     </row>
-    <row r="23" spans="1:15" ht="15.95" customHeight="1">
+    <row r="23" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="10" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="B23" s="11">
-        <v>1000</v>
+        <v>995</v>
       </c>
       <c r="C23" s="4">
-        <v>1090</v>
+        <v>1075</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -2128,28 +2174,28 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="10" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="J23" s="13">
-        <v>3710</v>
+        <v>4015</v>
       </c>
       <c r="K23" s="4">
-        <v>3990</v>
+        <v>4390</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
     </row>
-    <row r="24" spans="1:15" ht="15.95" customHeight="1">
+    <row r="24" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="10" t="s">
-        <v>43</v>
+        <v>102</v>
       </c>
       <c r="B24" s="11">
-        <v>960</v>
+        <v>880</v>
       </c>
       <c r="C24" s="4">
-        <v>1040</v>
+        <v>950</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -2157,28 +2203,28 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="10" t="s">
-        <v>92</v>
+        <v>21</v>
       </c>
       <c r="J24" s="13">
-        <v>3620</v>
+        <v>3710</v>
       </c>
       <c r="K24" s="4">
-        <v>3890</v>
+        <v>3990</v>
       </c>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
     </row>
-    <row r="25" spans="1:15" ht="15.95" customHeight="1">
+    <row r="25" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B25" s="11">
+        <v>960</v>
+      </c>
+      <c r="C25" s="4">
         <v>1040</v>
-      </c>
-      <c r="C25" s="4">
-        <v>1120</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -2186,28 +2232,28 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="10" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="J25" s="13">
-        <v>4620</v>
+        <v>3620</v>
       </c>
       <c r="K25" s="4">
-        <v>4999</v>
+        <v>3890</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
     </row>
-    <row r="26" spans="1:15" ht="15.95" customHeight="1">
+    <row r="26" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="10" t="s">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="B26" s="11">
-        <v>930</v>
+        <v>1040</v>
       </c>
       <c r="C26" s="4">
-        <v>999</v>
+        <v>1120</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -2215,28 +2261,28 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="10" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J26" s="13">
-        <v>4520</v>
+        <v>4620</v>
       </c>
       <c r="K26" s="4">
-        <v>4899</v>
+        <v>4999</v>
       </c>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
     </row>
-    <row r="27" spans="1:15" ht="15.95" customHeight="1">
+    <row r="27" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="10" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="B27" s="11">
-        <v>1290</v>
+        <v>930</v>
       </c>
       <c r="C27" s="4">
-        <v>1390</v>
+        <v>999</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -2244,28 +2290,28 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="10" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="J27" s="13">
-        <v>4080</v>
+        <v>4520</v>
       </c>
       <c r="K27" s="4">
-        <v>4390</v>
+        <v>4899</v>
       </c>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
     </row>
-    <row r="28" spans="1:15" ht="15.95" customHeight="1">
+    <row r="28" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A28" s="10" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B28" s="11">
-        <v>1190</v>
+        <v>1290</v>
       </c>
       <c r="C28" s="4">
-        <v>1290</v>
+        <v>1390</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -2273,28 +2319,28 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="14" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="J28" s="13">
-        <v>4220</v>
+        <v>4080</v>
       </c>
       <c r="K28" s="4">
-        <v>4540</v>
+        <v>4390</v>
       </c>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
     </row>
-    <row r="29" spans="1:15" ht="15.95" customHeight="1">
+    <row r="29" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A29" s="10" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="B29" s="11">
-        <v>1270</v>
+        <v>1190</v>
       </c>
       <c r="C29" s="4">
-        <v>1370</v>
+        <v>1290</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -2302,28 +2348,28 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="14" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="J29" s="13">
-        <v>12240</v>
+        <v>4220</v>
       </c>
       <c r="K29" s="4">
-        <v>12990</v>
+        <v>4540</v>
       </c>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
     </row>
-    <row r="30" spans="1:15" ht="15.95" customHeight="1">
+    <row r="30" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A30" s="10" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="B30" s="11">
-        <v>1170</v>
+        <v>1270</v>
       </c>
       <c r="C30" s="4">
-        <v>1270</v>
+        <v>1370</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -2331,10 +2377,10 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J30" s="15">
-        <v>12090</v>
+        <v>12240</v>
       </c>
       <c r="K30" s="4">
         <v>12990</v>
@@ -2344,15 +2390,15 @@
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
     </row>
-    <row r="31" spans="1:15" ht="15.95" customHeight="1">
+    <row r="31" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A31" s="10" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="B31" s="11">
-        <v>1190</v>
+        <v>1170</v>
       </c>
       <c r="C31" s="4">
-        <v>1290</v>
+        <v>1270</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -2360,28 +2406,28 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J31" s="15">
-        <v>10840</v>
+        <v>12090</v>
       </c>
       <c r="K31" s="4">
-        <v>11990</v>
+        <v>12990</v>
       </c>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
     </row>
-    <row r="32" spans="1:15" ht="15.95" customHeight="1">
+    <row r="32" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A32" s="10" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="B32" s="11">
-        <v>1225</v>
+        <v>1190</v>
       </c>
       <c r="C32" s="4">
-        <v>1325</v>
+        <v>1290</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -2389,28 +2435,28 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J32" s="15">
-        <v>12490</v>
+        <v>10840</v>
       </c>
       <c r="K32" s="4">
-        <v>13490</v>
+        <v>11990</v>
       </c>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
     </row>
-    <row r="33" spans="1:15" ht="15.95" customHeight="1">
+    <row r="33" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A33" s="10" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="B33" s="11">
-        <v>1220</v>
+        <v>1225</v>
       </c>
       <c r="C33" s="4">
-        <v>1320</v>
+        <v>1325</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -2418,51 +2464,57 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="12" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="J33" s="13">
-        <v>8820</v>
+        <v>12490</v>
       </c>
       <c r="K33" s="4">
-        <v>9490</v>
+        <v>13490</v>
       </c>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
     </row>
-    <row r="34" spans="1:15" ht="15.95" customHeight="1">
+    <row r="34" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A34" s="10" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B34" s="11">
-        <v>1080</v>
+        <v>1220</v>
       </c>
       <c r="C34" s="4">
-        <v>1160</v>
+        <v>1320</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="4"/>
+      <c r="I34" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="J34" s="15">
+        <v>8820</v>
+      </c>
+      <c r="K34" s="4">
+        <v>9490</v>
+      </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
     </row>
-    <row r="35" spans="1:15" ht="15.95" customHeight="1">
+    <row r="35" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A35" s="10" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B35" s="11">
-        <v>1100</v>
+        <v>1080</v>
       </c>
       <c r="C35" s="4">
-        <v>1199</v>
+        <v>1160</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -2477,15 +2529,15 @@
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
     </row>
-    <row r="36" spans="1:15" ht="15.95" customHeight="1">
+    <row r="36" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A36" s="10" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="B36" s="16">
-        <v>1200</v>
+        <v>1100</v>
       </c>
       <c r="C36" s="4">
-        <v>1290</v>
+        <v>1199</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -2500,15 +2552,15 @@
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
     </row>
-    <row r="37" spans="1:15" ht="15.95" customHeight="1">
+    <row r="37" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A37" s="10" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B37" s="11">
-        <v>1120</v>
+        <v>1200</v>
       </c>
       <c r="C37" s="4">
-        <v>1220</v>
+        <v>1290</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -2523,15 +2575,15 @@
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
     </row>
-    <row r="38" spans="1:15" ht="15.95" customHeight="1">
+    <row r="38" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A38" s="10" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B38" s="11">
-        <v>1040</v>
+        <v>1120</v>
       </c>
       <c r="C38" s="4">
-        <v>1130</v>
+        <v>1220</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -2546,15 +2598,15 @@
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
     </row>
-    <row r="39" spans="1:15" ht="15.95" customHeight="1">
+    <row r="39" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A39" s="10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B39" s="11">
-        <v>1100</v>
+        <v>1040</v>
       </c>
       <c r="C39" s="4">
-        <v>1199</v>
+        <v>1130</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -2569,9 +2621,9 @@
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
     </row>
-    <row r="40" spans="1:15" ht="15.95" customHeight="1">
+    <row r="40" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A40" s="10" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B40" s="11">
         <v>1100</v>
@@ -2592,15 +2644,15 @@
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
     </row>
-    <row r="41" spans="1:15" ht="15.95" customHeight="1">
+    <row r="41" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A41" s="10" t="s">
-        <v>66</v>
+        <v>4</v>
       </c>
       <c r="B41" s="11">
-        <v>1050</v>
+        <v>1100</v>
       </c>
       <c r="C41" s="4">
-        <v>1130</v>
+        <v>1199</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -2615,15 +2667,15 @@
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
     </row>
-    <row r="42" spans="1:15" ht="15.95" customHeight="1">
+    <row r="42" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A42" s="10" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="B42" s="11">
+        <v>1050</v>
+      </c>
+      <c r="C42" s="4">
         <v>1130</v>
-      </c>
-      <c r="C42" s="4">
-        <v>1230</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -2638,15 +2690,15 @@
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
     </row>
-    <row r="43" spans="1:15" ht="15.95" customHeight="1">
+    <row r="43" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A43" s="10" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B43" s="11">
-        <v>1100</v>
+        <v>1130</v>
       </c>
       <c r="C43" s="4">
-        <v>1190</v>
+        <v>1230</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -2661,88 +2713,88 @@
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
     </row>
-    <row r="44" spans="1:15" ht="15.95" customHeight="1">
+    <row r="44" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A44" s="10" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="B44" s="11">
-        <v>1330</v>
+        <v>1100</v>
       </c>
       <c r="C44" s="4">
-        <v>1450</v>
+        <v>1190</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-      <c r="I44" s="30" t="s">
+      <c r="I44" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="39"/>
+      <c r="J44" s="33"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="30"/>
-      <c r="N44" s="30"/>
+      <c r="M44" s="32"/>
+      <c r="N44" s="32"/>
       <c r="O44" s="17"/>
     </row>
-    <row r="45" spans="1:15" ht="15.95" customHeight="1">
+    <row r="45" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A45" s="10" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="B45" s="11">
-        <v>1200</v>
+        <v>1330</v>
       </c>
       <c r="C45" s="4">
-        <v>1299</v>
+        <v>1450</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
-      <c r="K45" s="30"/>
-      <c r="L45" s="30"/>
-      <c r="M45" s="30"/>
-      <c r="N45" s="30"/>
-      <c r="O45" s="30"/>
-    </row>
-    <row r="46" spans="1:15" ht="15.95" customHeight="1">
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="32"/>
+      <c r="L45" s="32"/>
+      <c r="M45" s="32"/>
+      <c r="N45" s="32"/>
+      <c r="O45" s="32"/>
+    </row>
+    <row r="46" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A46" s="10" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B46" s="11">
-        <v>1250</v>
+        <v>1200</v>
       </c>
       <c r="C46" s="4">
-        <v>1350</v>
+        <v>1299</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="31" t="s">
+      <c r="I46" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="31"/>
-      <c r="K46" s="31"/>
-      <c r="L46" s="31"/>
-      <c r="M46" s="31"/>
-      <c r="N46" s="31"/>
-      <c r="O46" s="32"/>
-    </row>
-    <row r="47" spans="1:15" ht="15.95" customHeight="1">
+      <c r="J46" s="40"/>
+      <c r="K46" s="40"/>
+      <c r="L46" s="40"/>
+      <c r="M46" s="40"/>
+      <c r="N46" s="40"/>
+      <c r="O46" s="41"/>
+    </row>
+    <row r="47" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A47" s="10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B47" s="11">
-        <v>1370</v>
+        <v>1250</v>
       </c>
       <c r="C47" s="4">
-        <v>1490</v>
+        <v>1350</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
@@ -2755,23 +2807,23 @@
       <c r="J47" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="30" t="s">
+      <c r="K47" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="30"/>
-      <c r="M47" s="30"/>
-      <c r="N47" s="30"/>
-      <c r="O47" s="33"/>
-    </row>
-    <row r="48" spans="1:15" ht="15.95" customHeight="1">
+      <c r="L47" s="32"/>
+      <c r="M47" s="32"/>
+      <c r="N47" s="32"/>
+      <c r="O47" s="42"/>
+    </row>
+    <row r="48" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A48" s="10" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="B48" s="11">
-        <v>2780</v>
+        <v>1370</v>
       </c>
       <c r="C48" s="4">
-        <v>2990</v>
+        <v>1490</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -2786,17 +2838,17 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="33"/>
-    </row>
-    <row r="49" spans="1:15" ht="15.95" customHeight="1">
+      <c r="O48" s="42"/>
+    </row>
+    <row r="49" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A49" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B49" s="11">
-        <v>6540</v>
+        <v>2780</v>
       </c>
       <c r="C49" s="4">
-        <v>6990</v>
+        <v>2990</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -2811,17 +2863,17 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="33"/>
-    </row>
-    <row r="50" spans="1:15" ht="15.95" customHeight="1">
+      <c r="O49" s="42"/>
+    </row>
+    <row r="50" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A50" s="4" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="B50" s="4">
-        <v>5290</v>
+        <v>6540</v>
       </c>
       <c r="C50" s="4">
-        <v>5690</v>
+        <v>6990</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -2836,17 +2888,17 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="33"/>
-    </row>
-    <row r="51" spans="1:15" ht="15.95" customHeight="1">
+      <c r="O50" s="42"/>
+    </row>
+    <row r="51" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A51" s="4" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="B51" s="4">
-        <v>5470</v>
+        <v>5290</v>
       </c>
       <c r="C51" s="4">
-        <v>5890</v>
+        <v>5690</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -2861,17 +2913,17 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="33"/>
-    </row>
-    <row r="52" spans="1:15" ht="15.95" customHeight="1">
+      <c r="O51" s="42"/>
+    </row>
+    <row r="52" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A52" s="4" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="B52" s="4">
-        <v>5750</v>
+        <v>5470</v>
       </c>
       <c r="C52" s="4">
-        <v>6190</v>
+        <v>5890</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -2886,17 +2938,17 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="33"/>
-    </row>
-    <row r="53" spans="1:15" ht="15.95" customHeight="1">
+      <c r="O52" s="42"/>
+    </row>
+    <row r="53" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A53" s="4" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B53" s="4">
-        <v>5940</v>
+        <v>5750</v>
       </c>
       <c r="C53" s="4">
-        <v>6390</v>
+        <v>6190</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -2911,17 +2963,17 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="33"/>
-    </row>
-    <row r="54" spans="1:15" ht="15.95" customHeight="1">
+      <c r="O53" s="42"/>
+    </row>
+    <row r="54" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A54" s="4" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="B54" s="4">
-        <v>6530</v>
+        <v>5940</v>
       </c>
       <c r="C54" s="4">
-        <v>6990</v>
+        <v>6390</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -2936,17 +2988,17 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="33"/>
-    </row>
-    <row r="55" spans="1:15" ht="15.95" customHeight="1">
+      <c r="O54" s="42"/>
+    </row>
+    <row r="55" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A55" s="4" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="B55" s="4">
-        <v>8340</v>
+        <v>6530</v>
       </c>
       <c r="C55" s="4">
-        <v>8990</v>
+        <v>6990</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -2961,17 +3013,17 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="33"/>
-    </row>
-    <row r="56" spans="1:15" ht="15.95" customHeight="1">
+      <c r="O55" s="42"/>
+    </row>
+    <row r="56" spans="1:15" ht="17.100000000000001" customHeight="1">
       <c r="A56" s="10" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="B56" s="10">
-        <v>9190</v>
+        <v>8340</v>
       </c>
       <c r="C56" s="10">
-        <v>9990</v>
+        <v>8990</v>
       </c>
       <c r="D56" s="10"/>
       <c r="E56" s="10"/>
@@ -2986,7 +3038,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="34"/>
+      <c r="O56" s="43"/>
     </row>
     <row r="57" spans="1:15" ht="16.5" thickBot="1">
       <c r="A57" s="18"/>
@@ -3006,49 +3058,49 @@
       <c r="O57" s="22"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="28" t="s">
+      <c r="A58" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="28"/>
-      <c r="C58" s="28"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="38"/>
       <c r="D58" s="23"/>
       <c r="E58" s="24"/>
-      <c r="F58" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="G58" s="46"/>
-      <c r="H58" s="46"/>
-      <c r="I58" s="46"/>
-      <c r="J58" s="46"/>
-      <c r="K58" s="47"/>
+      <c r="F58" s="51"/>
+      <c r="G58" s="52" t="s">
+        <v>106</v>
+      </c>
+      <c r="H58" s="53"/>
+      <c r="I58" s="54"/>
+      <c r="J58" s="51"/>
+      <c r="K58" s="51"/>
       <c r="L58" s="23"/>
       <c r="M58" s="24"/>
-      <c r="N58" s="29" t="s">
+      <c r="N58" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="29"/>
+      <c r="O58" s="45"/>
     </row>
     <row r="59" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A59" s="38"/>
-      <c r="B59" s="38"/>
-      <c r="C59" s="38"/>
+      <c r="A59" s="31"/>
+      <c r="B59" s="31"/>
+      <c r="C59" s="31"/>
       <c r="D59" s="20"/>
       <c r="E59" s="18"/>
-      <c r="F59" s="48"/>
-      <c r="G59" s="49"/>
-      <c r="H59" s="49"/>
-      <c r="I59" s="49"/>
-      <c r="J59" s="49"/>
-      <c r="K59" s="50"/>
+      <c r="F59" s="51"/>
+      <c r="G59" s="55"/>
+      <c r="H59" s="56"/>
+      <c r="I59" s="57"/>
+      <c r="J59" s="51"/>
+      <c r="K59" s="51"/>
       <c r="L59" s="20"/>
       <c r="M59" s="18"/>
-      <c r="N59" s="38"/>
-      <c r="O59" s="38"/>
+      <c r="N59" s="31"/>
+      <c r="O59" s="31"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="38"/>
-      <c r="B60" s="38"/>
-      <c r="C60" s="38"/>
+      <c r="A60" s="31"/>
+      <c r="B60" s="31"/>
+      <c r="C60" s="31"/>
       <c r="D60" s="20"/>
       <c r="E60" s="18"/>
       <c r="F60" s="18"/>
@@ -3059,15 +3111,13 @@
       <c r="K60" s="20"/>
       <c r="L60" s="20"/>
       <c r="M60" s="18"/>
-      <c r="N60" s="38"/>
-      <c r="O60" s="38"/>
+      <c r="N60" s="31"/>
+      <c r="O60" s="31"/>
     </row>
     <row r="61" spans="1:15">
-      <c r="A61" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="B61" s="28"/>
-      <c r="C61" s="28"/>
+      <c r="A61" s="24"/>
+      <c r="B61" s="24"/>
+      <c r="C61" s="24"/>
       <c r="D61" s="23"/>
       <c r="E61" s="23"/>
       <c r="F61" s="23"/>
@@ -3078,11 +3128,18 @@
       <c r="K61" s="23"/>
       <c r="L61" s="23"/>
       <c r="M61" s="27"/>
-      <c r="N61" s="29"/>
-      <c r="O61" s="29"/>
+      <c r="N61" s="27"/>
+      <c r="O61" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="18">
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="N58:O58"/>
+    <mergeCell ref="G58:I59"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="K1:O1"/>
     <mergeCell ref="A1:E1"/>
@@ -3094,15 +3151,6 @@
     <mergeCell ref="A3:O3"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="A4:D4"/>
-    <mergeCell ref="F58:K59"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="N61:O61"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="N58:O58"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.3" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3138,73 +3186,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="35" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="36" t="s">
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
     </row>
     <row r="3" spans="1:15" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -3212,12 +3260,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="42" t="s">
+      <c r="L4" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1">
       <c r="A5" s="7" t="s">
@@ -4321,14 +4369,14 @@
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
-      <c r="I44" s="30" t="s">
+      <c r="I44" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="39"/>
+      <c r="J44" s="33"/>
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
-      <c r="M44" s="30"/>
-      <c r="N44" s="30"/>
+      <c r="M44" s="32"/>
+      <c r="N44" s="32"/>
       <c r="O44" s="17"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1">
@@ -4346,13 +4394,13 @@
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
-      <c r="K45" s="30"/>
-      <c r="L45" s="30"/>
-      <c r="M45" s="30"/>
-      <c r="N45" s="30"/>
-      <c r="O45" s="30"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="32"/>
+      <c r="L45" s="32"/>
+      <c r="M45" s="32"/>
+      <c r="N45" s="32"/>
+      <c r="O45" s="32"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1">
       <c r="A46" s="10" t="s">
@@ -4369,15 +4417,15 @@
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
-      <c r="I46" s="31" t="s">
+      <c r="I46" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="31"/>
-      <c r="K46" s="31"/>
-      <c r="L46" s="31"/>
-      <c r="M46" s="31"/>
-      <c r="N46" s="31"/>
-      <c r="O46" s="32"/>
+      <c r="J46" s="40"/>
+      <c r="K46" s="40"/>
+      <c r="L46" s="40"/>
+      <c r="M46" s="40"/>
+      <c r="N46" s="40"/>
+      <c r="O46" s="41"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1">
       <c r="A47" s="10" t="s">
@@ -4400,13 +4448,13 @@
       <c r="J47" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="30" t="s">
+      <c r="K47" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="30"/>
-      <c r="M47" s="30"/>
-      <c r="N47" s="30"/>
-      <c r="O47" s="33"/>
+      <c r="L47" s="32"/>
+      <c r="M47" s="32"/>
+      <c r="N47" s="32"/>
+      <c r="O47" s="42"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1">
       <c r="A48" s="10" t="s">
@@ -4431,7 +4479,7 @@
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
       <c r="N48" s="5"/>
-      <c r="O48" s="33"/>
+      <c r="O48" s="42"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1">
       <c r="A49" s="10" t="s">
@@ -4456,7 +4504,7 @@
       <c r="L49" s="5"/>
       <c r="M49" s="5"/>
       <c r="N49" s="5"/>
-      <c r="O49" s="33"/>
+      <c r="O49" s="42"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1">
       <c r="A50" s="5" t="s">
@@ -4481,7 +4529,7 @@
       <c r="L50" s="5"/>
       <c r="M50" s="5"/>
       <c r="N50" s="5"/>
-      <c r="O50" s="33"/>
+      <c r="O50" s="42"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1">
       <c r="A51" s="5" t="s">
@@ -4506,7 +4554,7 @@
       <c r="L51" s="5"/>
       <c r="M51" s="5"/>
       <c r="N51" s="5"/>
-      <c r="O51" s="33"/>
+      <c r="O51" s="42"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1">
       <c r="A52" s="5" t="s">
@@ -4531,7 +4579,7 @@
       <c r="L52" s="5"/>
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
-      <c r="O52" s="33"/>
+      <c r="O52" s="42"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1">
       <c r="A53" s="5" t="s">
@@ -4556,7 +4604,7 @@
       <c r="L53" s="5"/>
       <c r="M53" s="5"/>
       <c r="N53" s="5"/>
-      <c r="O53" s="33"/>
+      <c r="O53" s="42"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1">
       <c r="A54" s="5" t="s">
@@ -4581,7 +4629,7 @@
       <c r="L54" s="5"/>
       <c r="M54" s="5"/>
       <c r="N54" s="5"/>
-      <c r="O54" s="33"/>
+      <c r="O54" s="42"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1">
       <c r="A55" s="5" t="s">
@@ -4606,7 +4654,7 @@
       <c r="L55" s="5"/>
       <c r="M55" s="5"/>
       <c r="N55" s="5"/>
-      <c r="O55" s="33"/>
+      <c r="O55" s="42"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1">
       <c r="A56" s="10" t="s">
@@ -4631,7 +4679,7 @@
       <c r="L56" s="5"/>
       <c r="M56" s="5"/>
       <c r="N56" s="5"/>
-      <c r="O56" s="34"/>
+      <c r="O56" s="43"/>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="18"/>
@@ -4651,11 +4699,11 @@
       <c r="O57" s="22"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="28" t="s">
+      <c r="A58" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="28"/>
-      <c r="C58" s="28"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="38"/>
       <c r="D58" s="23"/>
       <c r="E58" s="24"/>
       <c r="F58" s="44" t="s">
@@ -4668,15 +4716,15 @@
       <c r="K58" s="44"/>
       <c r="L58" s="23"/>
       <c r="M58" s="24"/>
-      <c r="N58" s="29" t="s">
+      <c r="N58" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="29"/>
+      <c r="O58" s="39"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="38"/>
-      <c r="B59" s="38"/>
-      <c r="C59" s="38"/>
+      <c r="A59" s="31"/>
+      <c r="B59" s="31"/>
+      <c r="C59" s="31"/>
       <c r="D59" s="25"/>
       <c r="E59" s="18"/>
       <c r="F59" s="44"/>
@@ -4687,13 +4735,13 @@
       <c r="K59" s="44"/>
       <c r="L59" s="25"/>
       <c r="M59" s="18"/>
-      <c r="N59" s="38"/>
-      <c r="O59" s="38"/>
+      <c r="N59" s="31"/>
+      <c r="O59" s="31"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="38"/>
-      <c r="B60" s="38"/>
-      <c r="C60" s="38"/>
+      <c r="A60" s="31"/>
+      <c r="B60" s="31"/>
+      <c r="C60" s="31"/>
       <c r="D60" s="25"/>
       <c r="E60" s="18"/>
       <c r="F60" s="18"/>
@@ -4704,15 +4752,15 @@
       <c r="K60" s="25"/>
       <c r="L60" s="25"/>
       <c r="M60" s="18"/>
-      <c r="N60" s="38"/>
-      <c r="O60" s="38"/>
+      <c r="N60" s="31"/>
+      <c r="O60" s="31"/>
     </row>
     <row r="61" spans="1:15">
-      <c r="A61" s="28" t="s">
+      <c r="A61" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="28"/>
-      <c r="C61" s="28"/>
+      <c r="B61" s="38"/>
+      <c r="C61" s="38"/>
       <c r="D61" s="23"/>
       <c r="E61" s="23"/>
       <c r="F61" s="23"/>
@@ -4723,11 +4771,24 @@
       <c r="K61" s="23"/>
       <c r="L61" s="23"/>
       <c r="M61" s="27"/>
-      <c r="N61" s="29"/>
-      <c r="O61" s="29"/>
+      <c r="N61" s="39"/>
+      <c r="O61" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="N58:O58"/>
     <mergeCell ref="A59:C60"/>
@@ -4735,19 +4796,6 @@
     <mergeCell ref="A61:C61"/>
     <mergeCell ref="N61:O61"/>
     <mergeCell ref="F58:K59"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>